<commit_message>
Latest code with Allure and Extent Reports
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajas\eclipse-workspace\webautomationdemo-main\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A098067-3198-4217-89FC-65F7DCD8D153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD19477-A9B7-4340-9A87-68F566A5A3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>searchtext</t>
   </si>
   <si>
-    <t>Automation Anywhere</t>
+    <t>Katalon Studio</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Latest code with Jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajas\eclipse-workspace\webautomationdemo-main\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD19477-A9B7-4340-9A87-68F566A5A3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98C6C7E-A4B7-4ACC-B66A-CA7CBFB3BAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Katalon Studio</t>
+  </si>
+  <si>
+    <t>yuva</t>
+  </si>
+  <si>
+    <t>Automation Anywhere</t>
   </si>
 </sst>
 </file>
@@ -357,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,6 +396,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>